<commit_message>
Canges to "A" related files
</commit_message>
<xml_diff>
--- a/statistics_files/2023/executive_board/2023_02_next_statistics.xlsx
+++ b/statistics_files/2023/executive_board/2023_02_next_statistics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\executive_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390371DE-1C15-454C-A7EB-2F1A902E9BA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B45BC70-9C7D-414E-985A-1458CB61040E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{76F7C32B-939B-4119-B411-60C078B28972}"/>
   </bookViews>
@@ -719,7 +719,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,457 +756,799 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="5">
+        <v>11206</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1834</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1972</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="7">
+        <v>5732</v>
+      </c>
+      <c r="C4" s="7">
+        <v>720</v>
+      </c>
+      <c r="D4" s="7">
+        <v>765</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5">
+        <v>18905</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1757</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1800</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="7">
+        <v>226</v>
+      </c>
+      <c r="C6" s="7">
+        <v>200</v>
+      </c>
+      <c r="D6" s="7">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="5">
+        <v>12027</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2090</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1933</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="B8" s="7">
+        <v>1522</v>
+      </c>
+      <c r="C8" s="7">
+        <v>352</v>
+      </c>
+      <c r="D8" s="7">
+        <v>371</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="5">
+        <v>1555</v>
+      </c>
+      <c r="C9" s="5">
+        <v>298</v>
+      </c>
+      <c r="D9" s="5">
+        <v>201</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="7">
+        <v>512</v>
+      </c>
+      <c r="C10" s="7">
+        <v>123</v>
+      </c>
+      <c r="D10" s="7">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="5">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5">
+        <v>65</v>
+      </c>
+      <c r="D11" s="5">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="7">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9">
+        <v>265</v>
+      </c>
+      <c r="C13" s="9">
+        <v>72</v>
+      </c>
+      <c r="D13" s="9">
+        <v>106</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
+      <c r="B14" s="11">
+        <v>841</v>
+      </c>
+      <c r="C14" s="11">
+        <v>366</v>
+      </c>
+      <c r="D14" s="11">
+        <v>200</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="B15" s="9">
+        <v>1498</v>
+      </c>
+      <c r="C15" s="9">
+        <v>555</v>
+      </c>
+      <c r="D15" s="9">
+        <v>237</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="B16" s="11">
+        <v>741</v>
+      </c>
+      <c r="C16" s="11">
+        <v>352</v>
+      </c>
+      <c r="D16" s="11">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="5">
+        <v>501</v>
+      </c>
+      <c r="C17" s="5">
+        <v>249</v>
+      </c>
+      <c r="D17" s="5">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="7">
+        <v>4066</v>
+      </c>
+      <c r="C18" s="7">
+        <v>831</v>
+      </c>
+      <c r="D18" s="7">
+        <v>856</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="5">
+        <v>463</v>
+      </c>
+      <c r="C19" s="5">
+        <v>208</v>
+      </c>
+      <c r="D19" s="5">
+        <v>168</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="B20" s="7">
+        <v>4937</v>
+      </c>
+      <c r="C20" s="7">
+        <v>575</v>
+      </c>
+      <c r="D20" s="7">
+        <v>899</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="5">
+        <v>79</v>
+      </c>
+      <c r="C21" s="5">
+        <v>107</v>
+      </c>
+      <c r="D21" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="7">
+        <v>4369</v>
+      </c>
+      <c r="C22" s="7">
+        <v>636</v>
+      </c>
+      <c r="D22" s="7">
+        <v>884</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5">
+        <v>347</v>
+      </c>
+      <c r="C23" s="5">
+        <v>117</v>
+      </c>
+      <c r="D23" s="5">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="7">
+        <v>4496</v>
+      </c>
+      <c r="C24" s="7">
+        <v>817</v>
+      </c>
+      <c r="D24" s="7">
+        <v>995</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="5">
+        <v>20866</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2075</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2607</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="7">
+        <v>1445</v>
+      </c>
+      <c r="C26" s="7">
+        <v>515</v>
+      </c>
+      <c r="D26" s="7">
+        <v>299</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="7">
+        <v>1357</v>
+      </c>
+      <c r="C28" s="7">
+        <v>284</v>
+      </c>
+      <c r="D28" s="7">
+        <v>287</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="5">
+        <v>353</v>
+      </c>
+      <c r="C29" s="5">
+        <v>152</v>
+      </c>
+      <c r="D29" s="5">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="7">
+        <v>4116</v>
+      </c>
+      <c r="C30" s="7">
+        <v>700</v>
+      </c>
+      <c r="D30" s="7">
+        <v>706</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="5">
+        <v>141</v>
+      </c>
+      <c r="C31" s="5">
+        <v>63</v>
+      </c>
+      <c r="D31" s="5">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="B32" s="7">
+        <v>635</v>
+      </c>
+      <c r="C32" s="7">
+        <v>512</v>
+      </c>
+      <c r="D32" s="7">
+        <v>78</v>
+      </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="5">
+        <v>4063</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1055</v>
+      </c>
+      <c r="D33" s="5">
+        <v>732</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="B34" s="7">
+        <v>2660</v>
+      </c>
+      <c r="C34" s="7">
+        <v>794</v>
+      </c>
+      <c r="D34" s="7">
+        <v>704</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="5">
+        <v>1646</v>
+      </c>
+      <c r="C35" s="5">
+        <v>178</v>
+      </c>
+      <c r="D35" s="5">
+        <v>390</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="B36" s="7">
+        <v>14304</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1632</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1467</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="5">
+        <v>1946</v>
+      </c>
+      <c r="C37" s="5">
+        <v>895</v>
+      </c>
+      <c r="D37" s="5">
+        <v>327</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="B38" s="7">
+        <v>6032</v>
+      </c>
+      <c r="C38" s="7">
+        <v>566</v>
+      </c>
+      <c r="D38" s="7">
+        <v>752</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="5">
+        <v>271</v>
+      </c>
+      <c r="C39" s="5">
+        <v>302</v>
+      </c>
+      <c r="D39" s="5">
+        <v>99</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
+      <c r="B40" s="7">
+        <v>454</v>
+      </c>
+      <c r="C40" s="7">
+        <v>167</v>
+      </c>
+      <c r="D40" s="7">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="13">
+        <v>878</v>
+      </c>
+      <c r="C41" s="13">
+        <v>133</v>
+      </c>
+      <c r="D41" s="13">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="15">
+        <v>4265</v>
+      </c>
+      <c r="C42" s="15">
+        <v>250</v>
+      </c>
+      <c r="D42" s="15">
+        <v>135</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
+      <c r="B43" s="13">
+        <v>154</v>
+      </c>
+      <c r="C43" s="13">
+        <v>33</v>
+      </c>
+      <c r="D43" s="13">
+        <v>52</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
+      <c r="B44" s="15">
+        <v>332</v>
+      </c>
+      <c r="C44" s="15">
+        <v>17</v>
+      </c>
+      <c r="D44" s="15">
+        <v>30</v>
+      </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
+      <c r="B45" s="13">
+        <v>594</v>
+      </c>
+      <c r="C45" s="13">
+        <v>14</v>
+      </c>
+      <c r="D45" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="B46" s="7">
+        <v>780</v>
+      </c>
+      <c r="C46" s="7">
+        <v>263</v>
+      </c>
+      <c r="D46" s="7">
+        <v>134</v>
+      </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="B47" s="5">
+        <v>2931</v>
+      </c>
+      <c r="C47" s="5">
+        <v>974</v>
+      </c>
+      <c r="D47" s="5">
+        <v>616</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
+      <c r="B48" s="7">
+        <v>8233</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1189</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1383</v>
+      </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="B49" s="5">
+        <v>3202</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1004</v>
+      </c>
+      <c r="D49" s="5">
+        <v>377</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
+      <c r="B50" s="7">
+        <v>3079</v>
+      </c>
+      <c r="C50" s="7">
+        <v>347</v>
+      </c>
+      <c r="D50" s="7">
+        <v>477</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="B51" s="5">
+        <v>7961</v>
+      </c>
+      <c r="C51" s="5">
+        <v>864</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1250</v>
+      </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
+      <c r="B52" s="7">
+        <v>1116</v>
+      </c>
+      <c r="C52" s="7">
+        <v>152</v>
+      </c>
+      <c r="D52" s="7">
+        <v>308</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="B53" s="5">
+        <v>3815</v>
+      </c>
+      <c r="C53" s="5">
+        <v>867</v>
+      </c>
+      <c r="D53" s="5">
+        <v>719</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="7">
+        <v>408</v>
+      </c>
+      <c r="C54" s="7">
+        <v>307</v>
+      </c>
+      <c r="D54" s="7">
+        <v>181</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="B55" s="5">
+        <v>568</v>
+      </c>
+      <c r="C55" s="5">
+        <v>416</v>
+      </c>
+      <c r="D55" s="5">
+        <v>52</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="B56" s="7">
+        <v>753</v>
+      </c>
+      <c r="C56" s="7">
+        <v>181</v>
+      </c>
+      <c r="D56" s="7">
+        <v>224</v>
+      </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
+      <c r="B57" s="17">
+        <v>3345</v>
+      </c>
+      <c r="C57" s="17">
+        <v>1345</v>
+      </c>
+      <c r="D57" s="17">
+        <v>639</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
+      <c r="B58" s="19">
+        <v>6223</v>
+      </c>
+      <c r="C58" s="19">
+        <v>447</v>
+      </c>
+      <c r="D58" s="19">
+        <v>286</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="21">
+        <v>173688</v>
+      </c>
+      <c r="C59" s="21">
+        <v>29225</v>
+      </c>
+      <c r="D59" s="21">
+        <v>26444</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:D2" xr:uid="{2BAA0360-28EA-43C5-949A-024CCEDC735A}"/>

</xml_diff>